<commit_message>
Updates and fixes * fix: same rule id repeats in summary for different attributes * fix: If one rule fails, don't fail others * update: message mapping refactored * update: test custom rule from outside library * update: unit tests and integration tests on Ktas sample data
</commit_message>
<xml_diff>
--- a/Non-Conformance-Report-Rules-v0.1.xlsx
+++ b/Non-Conformance-Report-Rules-v0.1.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$I$28</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$I$28</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -70,7 +70,7 @@
     <t xml:space="preserve">&lt;file-path&gt; doesn't follow naming format.</t>
   </si>
   <si>
-    <t xml:space="preserve">'^tbl_account_golden_gate_[\\d]{14}.csv$’</t>
+    <t xml:space="preserve">  '^tbl_account_golden_gate_[\\d]{14}.csv$’</t>
   </si>
   <si>
     <t xml:space="preserve">test_column1</t>
@@ -88,7 +88,7 @@
     <t xml:space="preserve">&lt;file-extension&gt; is not an accepted file type. Accepted file types are CSV, EXCEL.</t>
   </si>
   <si>
-    <t xml:space="preserve">'CSV', 'EXCEL'</t>
+    <t xml:space="preserve">  'CSV', 'EXCEL'</t>
   </si>
   <si>
     <t xml:space="preserve">Validates the file extension against the given list of extensions</t>
@@ -103,7 +103,7 @@
     <t xml:space="preserve">File header validation failed. Missing columns are &lt;missing-column-names&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">"test_column_1", "test_column_2"</t>
+    <t xml:space="preserve">  "test_column_1", "test_column_2"</t>
   </si>
   <si>
     <t xml:space="preserve">Validates the columns against given required columns</t>
@@ -187,7 +187,7 @@
     <t xml:space="preserve">test_column1 can contain value between 0 and 12 char long. &lt;test_column1-value&gt; is out of the limit.</t>
   </si>
   <si>
-    <t xml:space="preserve">0,12</t>
+    <t xml:space="preserve">  0,12</t>
   </si>
   <si>
     <t xml:space="preserve">Validates column value length is between given length</t>
@@ -205,7 +205,7 @@
     <t xml:space="preserve">'&lt;test_column1-value&gt;' does not match regex '^[a-zA-Z]$'</t>
   </si>
   <si>
-    <t xml:space="preserve">^[a-z]$</t>
+    <t xml:space="preserve">  ^[a-z]$</t>
   </si>
   <si>
     <t xml:space="preserve">Validates column value is matches with the given regular expression.</t>
@@ -214,7 +214,7 @@
     <t xml:space="preserve">'&lt;test_column2-value&gt;' does not match regex '^[a-zA-Z]$'</t>
   </si>
   <si>
-    <t xml:space="preserve">^[a-zA-Z]$</t>
+    <t xml:space="preserve">  ^[a-zA-Z]$</t>
   </si>
   <si>
     <t xml:space="preserve">CDP_AT_008 </t>
@@ -226,7 +226,7 @@
     <t xml:space="preserve">'&lt;test_column1-value&gt;' is not part of enum list ['TEST1', 'TEST2']</t>
   </si>
   <si>
-    <t xml:space="preserve">['TEST1', 'TEST2']</t>
+    <t xml:space="preserve">  ['TEST1', 'TEST2']</t>
   </si>
   <si>
     <t xml:space="preserve">Validates column value is one of the given enumerals</t>
@@ -235,7 +235,7 @@
     <t xml:space="preserve">'&lt;test_column2-value&gt;' is not part of enum list ['m', 'f']</t>
   </si>
   <si>
-    <t xml:space="preserve">['m', 'f']</t>
+    <t xml:space="preserve">  ['m', 'f']</t>
   </si>
   <si>
     <t xml:space="preserve">CDP_AT_009 </t>
@@ -247,7 +247,7 @@
     <t xml:space="preserve">'&lt;test_column1-value&gt;' does not follow date format "%d/%m/%Y"</t>
   </si>
   <si>
-    <t xml:space="preserve">"%d/%m/%Y"</t>
+    <t xml:space="preserve">  "%d/%m/%Y"</t>
   </si>
   <si>
     <t xml:space="preserve">Validates column value is matches with the given date format.</t>
@@ -271,13 +271,13 @@
     <t xml:space="preserve">KTAS-CONTACTS</t>
   </si>
   <si>
-    <t xml:space="preserve">'^tbl_contacts_golden_gate_[\\d]{14}.csv$’</t>
+    <t xml:space="preserve">  '^tbl_contacts_golden_gate_[\\d]{14}.csv$’</t>
   </si>
   <si>
     <t xml:space="preserve">XYZ</t>
   </si>
   <si>
-    <t xml:space="preserve">[‘XYZ’, ‘ABC’]</t>
+    <t xml:space="preserve">  [‘XYZ’, ‘ABC’]</t>
   </si>
   <si>
     <t xml:space="preserve">'&lt;XYZ-value&gt;' has to have valid value</t>
@@ -302,11 +302,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -327,6 +328,14 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -371,12 +380,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -392,65 +405,61 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="true">
+  <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="84.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="32.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="29.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="57.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="29.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="64.77"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="1" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -479,7 +488,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
@@ -508,7 +517,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -537,7 +546,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
@@ -551,7 +560,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>32</v>
       </c>
@@ -577,7 +586,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>32</v>
       </c>
@@ -600,7 +609,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>38</v>
       </c>
@@ -626,7 +635,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>38</v>
       </c>
@@ -649,7 +658,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>42</v>
       </c>
@@ -675,7 +684,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>42</v>
       </c>
@@ -724,7 +733,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>51</v>
       </c>
@@ -753,7 +762,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>51</v>
       </c>
@@ -779,7 +788,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>57</v>
       </c>
@@ -808,7 +817,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>57</v>
       </c>
@@ -834,7 +843,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>64</v>
       </c>
@@ -863,7 +872,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>64</v>
       </c>
@@ -918,7 +927,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>76</v>
       </c>
@@ -944,7 +953,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>76</v>
       </c>
@@ -967,7 +976,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>9</v>
       </c>
@@ -993,7 +1002,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>18</v>
       </c>
@@ -1019,7 +1028,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -1045,7 +1054,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>42</v>
       </c>
@@ -1068,7 +1077,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>42</v>
       </c>
@@ -1091,7 +1100,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>76</v>
       </c>
@@ -1114,7 +1123,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>76</v>
       </c>
@@ -1138,20 +1147,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I28">
-    <filterColumn colId="3">
-      <filters>
-        <filter val=""/>
-        <filter val="KTAS-VEHICLE"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Date"/>
-        <filter val="Date Format"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1159,6 +1154,5 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>